<commit_message>
new york sign glitch fixed
</commit_message>
<xml_diff>
--- a/example-output/xslx/NY_cafr2010-statement_of_activities.xlsx
+++ b/example-output/xslx/NY_cafr2010-statement_of_activities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="NY_cafr2010-statement_of_activi" sheetId="1" r:id="rId1"/>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0"/>
@@ -1601,7 +1601,7 @@
         <v>31075</v>
       </c>
       <c r="G46" s="12">
-        <v>27222</v>
+        <v>-27222</v>
       </c>
       <c r="H46" s="13">
         <v>3735</v>

</xml_diff>